<commit_message>
Generowany przebieg obiegow do excela
</commit_message>
<xml_diff>
--- a/src/inputs/plan_obiegow_taboru/plan_obiegow_taboru.xlsx
+++ b/src/inputs/plan_obiegow_taboru/plan_obiegow_taboru.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaspi\Documents\python\nowyObieg\v_1_0_1\src\inputs\plan_obiegow_taboru\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C351E3FB-1B39-4ADA-BDAB-85CF6A434765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301E63F7-9256-479C-85AC-32A38F8495D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="16">
   <si>
     <t>nr_obiegu</t>
   </si>
@@ -54,22 +65,25 @@
     <t>H</t>
   </si>
   <si>
-    <t>C-</t>
+    <t>B</t>
   </si>
   <si>
-    <t>(1-6)</t>
+    <t>[1-6]</t>
   </si>
   <si>
-    <t>H-</t>
+    <t>[7]</t>
   </si>
   <si>
-    <t>(2-5)</t>
+    <t>[1]</t>
   </si>
   <si>
-    <t>(1-4)</t>
+    <t>[2-5]</t>
   </si>
   <si>
-    <t>B</t>
+    <t>[1-4]</t>
+  </si>
+  <si>
+    <t>[5]</t>
   </si>
 </sst>
 </file>
@@ -105,8 +119,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -390,7 +405,7 @@
   <dimension ref="A1:F157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +530,7 @@
         <v>11639</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -529,7 +544,7 @@
         <v>11555</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1089,7 +1104,7 @@
         <v>6264</v>
       </c>
       <c r="D49" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1285,7 +1300,7 @@
         <v>5358</v>
       </c>
       <c r="D63" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1299,7 +1314,7 @@
         <v>6175</v>
       </c>
       <c r="D64" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1550,8 +1565,8 @@
       <c r="C82">
         <v>5450</v>
       </c>
-      <c r="D82">
-        <v>-7</v>
+      <c r="D82" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -1564,8 +1579,8 @@
       <c r="C83">
         <v>6299</v>
       </c>
-      <c r="D83">
-        <v>-7</v>
+      <c r="D83" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -1620,8 +1635,8 @@
       <c r="C87">
         <v>6185</v>
       </c>
-      <c r="D87">
-        <v>-7</v>
+      <c r="D87" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -1789,7 +1804,7 @@
         <v>11515</v>
       </c>
       <c r="D99" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -1803,7 +1818,7 @@
         <v>11531</v>
       </c>
       <c r="D100" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -1817,7 +1832,7 @@
         <v>11634</v>
       </c>
       <c r="D101" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -1831,7 +1846,7 @@
         <v>11553</v>
       </c>
       <c r="D102" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -1886,8 +1901,8 @@
       <c r="C106">
         <v>6294</v>
       </c>
-      <c r="D106">
-        <v>-7</v>
+      <c r="D106" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -1901,7 +1916,7 @@
         <v>11847</v>
       </c>
       <c r="D107" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -1915,7 +1930,7 @@
         <v>11813</v>
       </c>
       <c r="D108" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -1929,7 +1944,7 @@
         <v>11852</v>
       </c>
       <c r="D109" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -1943,7 +1958,7 @@
         <v>11816</v>
       </c>
       <c r="D110" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -2013,7 +2028,7 @@
         <v>11612</v>
       </c>
       <c r="D115" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -2027,7 +2042,7 @@
         <v>11909</v>
       </c>
       <c r="D116" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -2040,8 +2055,8 @@
       <c r="C117">
         <v>11610</v>
       </c>
-      <c r="D117">
-        <v>-1</v>
+      <c r="D117" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -2055,7 +2070,7 @@
         <v>11612</v>
       </c>
       <c r="D118" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -2069,7 +2084,7 @@
         <v>11915</v>
       </c>
       <c r="D119" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -2082,8 +2097,8 @@
       <c r="C120">
         <v>11916</v>
       </c>
-      <c r="D120">
-        <v>-5</v>
+      <c r="D120" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -2097,7 +2112,7 @@
         <v>11601</v>
       </c>
       <c r="D121" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -2111,7 +2126,7 @@
         <v>11812</v>
       </c>
       <c r="D122" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -2125,7 +2140,7 @@
         <v>11866</v>
       </c>
       <c r="D123" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -2139,7 +2154,7 @@
         <v>11823</v>
       </c>
       <c r="D124" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -2153,7 +2168,7 @@
         <v>11809</v>
       </c>
       <c r="D125" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -2209,7 +2224,7 @@
         <v>11684</v>
       </c>
       <c r="D129" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -2251,7 +2266,7 @@
         <v>12450</v>
       </c>
       <c r="D132" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -2377,7 +2392,7 @@
         <v>3463</v>
       </c>
       <c r="D141" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -2405,7 +2420,7 @@
         <v>11609</v>
       </c>
       <c r="D143" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -2419,7 +2434,7 @@
         <v>11848</v>
       </c>
       <c r="D144" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -2475,7 +2490,7 @@
         <v>11815</v>
       </c>
       <c r="D148" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -2573,7 +2588,7 @@
         <v>11685</v>
       </c>
       <c r="D155" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>